<commit_message>
register and login client using mongodb(mongoose)
</commit_message>
<xml_diff>
--- a/toDo.xlsx
+++ b/toDo.xlsx
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,6 +602,20 @@
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="D5" s="5">
+        <v>180</v>
+      </c>
+      <c r="E5" s="5">
+        <v>150</v>
+      </c>
+      <c r="F5" s="5">
+        <f>D5-E5</f>
+        <v>30</v>
+      </c>
+      <c r="G5" s="6">
+        <f>E5/(E5+F5)</f>
+        <v>0.83333333333333337</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -614,10 +628,10 @@
         <v>5</v>
       </c>
       <c r="D7" s="5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E7" s="5">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="F7" s="5">
         <v>0</v>
@@ -660,15 +674,14 @@
         <v>30</v>
       </c>
       <c r="E9" s="5">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F9" s="5">
-        <f>D9-E9</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G9" s="6">
         <f>E9/(E9+F9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
get all restaurant and get compared to restaurant
</commit_message>
<xml_diff>
--- a/toDo.xlsx
+++ b/toDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>Client</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Avancement</t>
+  </si>
+  <si>
+    <t>findRestaurant</t>
+  </si>
+  <si>
+    <t>findPlatByRestaurant</t>
   </si>
 </sst>
 </file>
@@ -543,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G49"/>
+  <dimension ref="A2:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,29 +714,29 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="5">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E11" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" ref="F11:F13" si="0">D11-E11</f>
-        <v>40</v>
+        <f>D11-E11</f>
+        <v>0</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" ref="G11:G13" si="1">E11/(E11+F11)</f>
-        <v>0</v>
+        <f>E11/(E11+F11)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
@@ -739,73 +745,85 @@
         <v>60</v>
       </c>
       <c r="E12" s="5">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <f t="shared" ref="F12:F14" si="0">D12-E12</f>
+        <v>20</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="G12:G14" si="1">E12/(E12+F12)</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="5">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="E13" s="5">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G13" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="B14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5">
+        <v>60</v>
+      </c>
+      <c r="E14" s="5">
+        <v>50</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="1"/>
+        <v>0.83333333333333337</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="B15" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
       </c>
       <c r="F15" s="5">
-        <f>D15+E15</f>
-        <v>30</v>
+        <f t="shared" ref="F15:F17" si="2">D15-E15</f>
+        <v>40</v>
       </c>
       <c r="G15" s="6">
-        <f>E15/(E15+F15)</f>
+        <f t="shared" ref="G15:G17" si="3">E15/(E15+F15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>6</v>
@@ -817,61 +835,48 @@
         <v>0</v>
       </c>
       <c r="F16" s="5">
-        <f>D16+E16</f>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="G16" s="6">
-        <f>E16/(E16+F16)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" s="5">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" ref="F17:F25" si="2">D17+E17</f>
-        <v>40</v>
+        <f t="shared" si="2"/>
+        <v>60</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" ref="G17:G25" si="3">E17/(E17+F17)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5">
-        <v>60</v>
-      </c>
-      <c r="E18" s="5">
-        <v>0</v>
-      </c>
-      <c r="F18" s="5">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="G18" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="B19" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
@@ -883,193 +888,193 @@
         <v>0</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="2"/>
+        <f>D19+E19</f>
         <v>30</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="3"/>
+        <f>E19/(E19+F19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5">
+        <v>60</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <f>D20+E20</f>
+        <v>60</v>
+      </c>
+      <c r="G20" s="6">
+        <f>E20/(E20+F20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>40</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" ref="F21:F29" si="4">D21+E21</f>
+        <v>40</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" ref="G21:G29" si="5">E21/(E21+F21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5">
+        <v>60</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="5">
-        <v>60</v>
-      </c>
-      <c r="E20" s="5">
-        <v>0</v>
-      </c>
-      <c r="F20" s="5">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="G20" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="C23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5">
+        <v>30</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="5">
+        <v>60</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="5">
+      <c r="C25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5">
         <v>20</v>
       </c>
-      <c r="E21" s="5">
-        <v>0</v>
-      </c>
-      <c r="F21" s="5">
-        <f t="shared" si="2"/>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="G21" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="G25" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="5">
+      <c r="C26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="5">
         <v>40</v>
       </c>
-      <c r="E22" s="5">
-        <v>0</v>
-      </c>
-      <c r="F22" s="5">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="G22" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="5">
-        <v>20</v>
-      </c>
-      <c r="E24" s="5">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="G24" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="5">
-        <v>60</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5">
-        <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="G25" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="5">
-        <v>30</v>
-      </c>
       <c r="E26" s="5">
         <v>0</v>
       </c>
       <c r="F26" s="5">
-        <f t="shared" ref="F26:F44" si="4">D26+E26</f>
-        <v>30</v>
-      </c>
-      <c r="G26" s="6">
-        <f t="shared" ref="G26:G44" si="5">E26/(E26+F26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="5">
-        <v>40</v>
-      </c>
-      <c r="E27" s="5">
-        <v>0</v>
-      </c>
-      <c r="F27" s="5">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G26" s="6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="6"/>
+    </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+      <c r="A28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="5">
         <v>20</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="5">
-        <v>60</v>
       </c>
       <c r="E28" s="5">
         <v>0</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="4"/>
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G28" s="6">
         <f t="shared" si="5"/>
@@ -1077,11 +1082,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>21</v>
+      <c r="B29" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D29" s="5">
         <v>60</v>
@@ -1099,96 +1104,96 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>22</v>
+      <c r="B30" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D30" s="5">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E30" s="5">
         <v>0</v>
       </c>
       <c r="F30" s="5">
-        <f t="shared" si="4"/>
-        <v>60</v>
+        <f t="shared" ref="F30:F48" si="6">D30+E30</f>
+        <v>30</v>
       </c>
       <c r="G30" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="G30:G48" si="7">E30/(E30+F30)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>23</v>
+      <c r="B31" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D31" s="5">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E31" s="5">
         <v>0</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" si="4"/>
-        <v>60</v>
+        <f t="shared" si="6"/>
+        <v>40</v>
       </c>
       <c r="G31" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D32" s="5">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E32" s="5">
         <v>0</v>
       </c>
       <c r="F32" s="5">
-        <f t="shared" si="4"/>
-        <v>40</v>
+        <f t="shared" si="6"/>
+        <v>60</v>
       </c>
       <c r="G32" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D33" s="5">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E33" s="5">
         <v>0</v>
       </c>
       <c r="F33" s="5">
-        <f t="shared" si="4"/>
-        <v>70</v>
+        <f t="shared" si="6"/>
+        <v>60</v>
       </c>
       <c r="G33" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>24</v>
@@ -1200,17 +1205,17 @@
         <v>0</v>
       </c>
       <c r="F34" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="G34" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>24</v>
@@ -1222,306 +1227,394 @@
         <v>0</v>
       </c>
       <c r="F35" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="G35" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="5">
+        <v>40</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="G36" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="5">
+        <v>70</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+      <c r="G37" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="5">
+        <v>60</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="G38" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="5">
+        <v>60</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="G39" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="5">
-        <v>60</v>
-      </c>
-      <c r="E36" s="5">
-        <v>0</v>
-      </c>
-      <c r="F36" s="5">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="G36" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+      <c r="D40" s="5">
+        <v>60</v>
+      </c>
+      <c r="E40" s="5">
+        <v>0</v>
+      </c>
+      <c r="F40" s="5">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="G40" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="5">
-        <v>60</v>
-      </c>
-      <c r="E37" s="5">
-        <v>0</v>
-      </c>
-      <c r="F37" s="5">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="G37" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="3" t="s">
+      <c r="D41" s="5">
+        <v>60</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="G41" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="5">
+      <c r="C42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="5">
         <v>40</v>
       </c>
-      <c r="E38" s="5">
-        <v>0</v>
-      </c>
-      <c r="F38" s="5">
-        <f t="shared" si="4"/>
+      <c r="E42" s="5">
+        <v>0</v>
+      </c>
+      <c r="F42" s="5">
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="G38" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="3" t="s">
+      <c r="G42" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="5">
+      <c r="C43" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="5">
         <v>40</v>
       </c>
-      <c r="E39" s="5">
-        <v>0</v>
-      </c>
-      <c r="F39" s="5">
-        <f t="shared" si="4"/>
+      <c r="E43" s="5">
+        <v>0</v>
+      </c>
+      <c r="F43" s="5">
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="G39" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="5">
-        <v>30</v>
-      </c>
-      <c r="E40" s="5">
-        <v>0</v>
-      </c>
-      <c r="F40" s="5">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="G40" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="5">
-        <v>30</v>
-      </c>
-      <c r="E41" s="5">
-        <v>0</v>
-      </c>
-      <c r="F41" s="5">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="G41" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="3" t="s">
+      <c r="G43" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="5">
+        <v>30</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+      <c r="F44" s="5">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="G44" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B45" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="5">
+        <v>30</v>
+      </c>
+      <c r="E45" s="5">
+        <v>0</v>
+      </c>
+      <c r="F45" s="5">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="G45" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B46" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="5">
-        <v>30</v>
-      </c>
-      <c r="E42" s="5">
-        <v>0</v>
-      </c>
-      <c r="F42" s="5">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="G42" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="3" t="s">
+      <c r="C46" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="5">
+        <v>30</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="G46" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="5">
-        <v>30</v>
-      </c>
-      <c r="E43" s="5">
-        <v>0</v>
-      </c>
-      <c r="F43" s="5">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="G43" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="3" t="s">
+      <c r="C47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="5">
+        <v>30</v>
+      </c>
+      <c r="E47" s="5">
+        <v>0</v>
+      </c>
+      <c r="F47" s="5">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="G47" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B48" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="5">
-        <v>60</v>
-      </c>
-      <c r="E44" s="5">
-        <v>0</v>
-      </c>
-      <c r="F44" s="5">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-      <c r="G44" s="6">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="6"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+      <c r="C48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="5">
+        <v>60</v>
+      </c>
+      <c r="E48" s="5">
+        <v>0</v>
+      </c>
+      <c r="F48" s="5">
+        <f t="shared" si="6"/>
+        <v>60</v>
+      </c>
+      <c r="G48" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B50" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="5">
+      <c r="C50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="5">
         <v>20</v>
       </c>
-      <c r="E46" s="5">
-        <v>0</v>
-      </c>
-      <c r="F46" s="5">
-        <f t="shared" ref="F46:F49" si="6">D46+E46</f>
+      <c r="E50" s="5">
+        <v>0</v>
+      </c>
+      <c r="F50" s="5">
+        <f t="shared" ref="F50:F53" si="8">D50+E50</f>
         <v>20</v>
       </c>
-      <c r="G46" s="6">
-        <f t="shared" ref="G46:G49" si="7">E46/(E46+F46)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
+      <c r="G50" s="6">
+        <f t="shared" ref="G50:G53" si="9">E50/(E50+F50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="5">
+      <c r="C51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="5">
         <v>20</v>
       </c>
-      <c r="E47" s="5">
-        <v>0</v>
-      </c>
-      <c r="F47" s="5">
-        <f t="shared" si="6"/>
+      <c r="E51" s="5">
+        <v>0</v>
+      </c>
+      <c r="F51" s="5">
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
-      <c r="G47" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="3" t="s">
+      <c r="G51" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="5">
-        <v>60</v>
-      </c>
-      <c r="E48" s="5">
-        <v>0</v>
-      </c>
-      <c r="F48" s="5">
-        <f t="shared" si="6"/>
-        <v>60</v>
-      </c>
-      <c r="G48" s="6">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="3" t="s">
+      <c r="C52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="5">
+        <v>60</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0</v>
+      </c>
+      <c r="F52" s="5">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="G52" s="6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="5">
+      <c r="C53" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="5">
         <v>50</v>
       </c>
-      <c r="E49" s="5">
-        <v>0</v>
-      </c>
-      <c r="F49" s="5">
-        <f t="shared" si="6"/>
+      <c r="E53" s="5">
+        <v>0</v>
+      </c>
+      <c r="F53" s="5">
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="G49" s="6">
-        <f t="shared" si="7"/>
+      <c r="G53" s="6">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>